<commit_message>
fixed xpath and updated data
</commit_message>
<xml_diff>
--- a/bin/testscripts/datatables/TC_01.xlsx
+++ b/bin/testscripts/datatables/TC_01.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rahul\eclipse-workspace\seleniumFramework\src\testscripts\datatables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\snapshot\seleniumFramework\src\testscripts\datatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -60,20 +60,34 @@
     <t>test@g.com</t>
   </si>
   <si>
-    <t>09/10/2017</t>
-  </si>
-  <si>
-    <t>09/24/2017</t>
-  </si>
-  <si>
     <t>TC_01</t>
+  </si>
+  <si>
+    <t>12/12/2017</t>
+  </si>
+  <si>
+    <t>12/24/2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -112,9 +126,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -457,68 +471,69 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625"/>
-    <col min="3" max="3" width="12.140625"/>
-    <col min="4" max="4" width="23.28515625"/>
-    <col min="5" max="5" width="11"/>
-    <col min="6" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="1"/>
+    <col min="3" max="3" width="12.140625" style="1"/>
+    <col min="4" max="4" width="23.28515625" style="1"/>
+    <col min="5" max="5" width="11" style="1"/>
+    <col min="6" max="1025" width="8.5703125" style="1"/>
+    <col min="1026" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>